<commit_message>
Added colours to mask
</commit_message>
<xml_diff>
--- a/experiment_log.xlsx
+++ b/experiment_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sk8717_ic_ac_uk/Documents/Documents/Year_4/FYP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sk8717_ic_ac_uk/Documents/Documents/Year_4/FYP/working/ImageSegmentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{D8AC6F0E-BDAB-4060-AD01-2ECBC7D0B7C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9BF87205-DFE5-4522-BE5A-73E220F07711}"/>
+  <xr:revisionPtr revIDLastSave="755" documentId="8_{D8AC6F0E-BDAB-4060-AD01-2ECBC7D0B7C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CE3923A-4F12-47A7-8F32-BFEAE2BE35EB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="20145" windowHeight="17040" xr2:uid="{3B8BE473-C074-4334-9039-55915628F2B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3B8BE473-C074-4334-9039-55915628F2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -220,12 +220,117 @@
   </si>
   <si>
     <t>0.3119</t>
+  </si>
+  <si>
+    <t>Yes - expontential decrease every epoch (0.8^epoch)</t>
+  </si>
+  <si>
+    <t>Implementing Akshays's code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- works
+</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>1 - CSP</t>
+  </si>
+  <si>
+    <t>2 - Grey Matter</t>
+  </si>
+  <si>
+    <t>-worse than 19</t>
+  </si>
+  <si>
+    <t>0 - Background
+1 - CSP
+2 - Grey Matter</t>
+  </si>
+  <si>
+    <t>- need to increase accuracy
+- dilates grey matter sections</t>
+  </si>
+  <si>
+    <t>0 - Background
+1 - CSP
+2 - Grey Matter
+3 - White Matter</t>
+  </si>
+  <si>
+    <t>- falsely recognises the area surrounding the brain as GM and WM</t>
+  </si>
+  <si>
+    <t>Yes - expontential decrease every epoch (0.9^epoch)</t>
+  </si>
+  <si>
+    <t>- lower loss than 24
+- looking at the images qualitatively: worse than 24
+- CSP is everywhere</t>
+  </si>
+  <si>
+    <t>1 - Background
+1 - CSP
+2 - Grey Matter
+3 - White Matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-trying multi-class for first time
+- img fed into model is shaped [img,0,0]
+- msk fed into model is shaped [background, CSP, GM]
+- recognises background
+- recognises 'everything in the brain' as grey matter
+- recognises contours of brain as CSP </t>
+  </si>
+  <si>
+    <t>-lower loss than 24
+-predicted mask is 'fuzzy'</t>
+  </si>
+  <si>
+    <t>0- Background
+1 - CSP
+2 - Grey Matter
+3 - White Matter
+4 - Fat</t>
+  </si>
+  <si>
+    <t>0 - Background
+1 - CSP
+2 - Grey Matter
+3 - White Matter
+4 - Fat
+5 - Muscle</t>
+  </si>
+  <si>
+    <t>-lower loss than 24
+- took very long to train</t>
+  </si>
+  <si>
+    <t>Mean accuracy (DICE)</t>
+  </si>
+  <si>
+    <t>- higher loss
+- predicts the entire area surrounding the brain to be fat
+- predicts CSP to be fat
+- predicts inside of brain to be white matter
+- predicts outline of brain to be grey matter</t>
+  </si>
+  <si>
+    <t>- lower accuracy
+- CSP, GM, WM look decently accurate
+- falsely predicted surroudning tissue to be fat
+- still dilation present</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -295,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -316,6 +421,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,13 +448,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>222582</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>703846</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>533401</xdr:rowOff>
@@ -384,13 +492,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>205846</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>529892</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
@@ -428,13 +536,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>212000</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>620093</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>381816</xdr:rowOff>
@@ -472,13 +580,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>3886200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>4958538</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>371475</xdr:rowOff>
@@ -516,13 +624,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>238124</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>75407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>572425</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>372297</xdr:rowOff>
@@ -560,13 +668,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>143794</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>82719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>632241</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>523874</xdr:rowOff>
@@ -604,13 +712,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>242950</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>583322</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>361949</xdr:rowOff>
@@ -648,13 +756,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>3933825</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>44800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>4895236</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>352229</xdr:rowOff>
@@ -692,13 +800,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>3629026</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>4686300</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>347608</xdr:rowOff>
@@ -736,13 +844,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>57972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>524830</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>1295</xdr:rowOff>
@@ -780,13 +888,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>100352</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>524787</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>324673</xdr:rowOff>
@@ -824,13 +932,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>247649</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>64156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>601018</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>372298</xdr:rowOff>
@@ -868,13 +976,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>72707</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>639093</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>514348</xdr:rowOff>
@@ -912,13 +1020,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>3585883</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>61438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>4448735</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>337350</xdr:rowOff>
@@ -956,13 +1064,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>246528</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>54419</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>558939</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>347655</xdr:rowOff>
@@ -990,6 +1098,1062 @@
         <a:xfrm>
           <a:off x="19453410" y="7315831"/>
           <a:ext cx="312411" cy="293236"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3305735</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47409</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4930588</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>547363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Grafik 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F29FDB64-DE11-49E8-8A28-02469B30D699}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20327470" y="8261321"/>
+          <a:ext cx="1624853" cy="499954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3300972</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>78440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4941909</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>8607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Grafik 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C55DBD04-C206-4497-8F3B-4AD857F7B350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19067648" y="8863852"/>
+          <a:ext cx="1640937" cy="501667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>31154</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>694766</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>528102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Grafik 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC631C0-EAAD-41EB-9CE0-3269C8C69E5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20798118" y="8816566"/>
+          <a:ext cx="649942" cy="496948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>94263</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>727473</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>554711</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Grafik 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E26F64B-4D89-4468-92D2-470ACC2BDF33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20847557" y="9435353"/>
+          <a:ext cx="633210" cy="476270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3395384</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4775501</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>512875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Grafik 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6959A66-46FB-4561-8713-46119D660BF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19162060" y="9447024"/>
+          <a:ext cx="1380117" cy="422763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3283325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>22213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4922854</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>531928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Grafik 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EC3038-8128-4051-87EE-2791CBCE31C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050001" y="9950625"/>
+          <a:ext cx="1639529" cy="509715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3260912</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4829849</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>543134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Grafik 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E97BFE3-4F07-4BEE-A4A8-058F6D26215D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19027588" y="10557202"/>
+          <a:ext cx="1568937" cy="485844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>58892</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>739070</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4939</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Grafik 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A50327B8-30E2-4E11-A5D6-B66AFD28AE62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20809323" y="10558804"/>
+          <a:ext cx="683041" cy="517547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3350558</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>336243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>111</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>829999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Grafik 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC090B05-3BFB-464F-923C-9CD0CAA893D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19117234" y="11407655"/>
+          <a:ext cx="1636171" cy="493756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28884</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>746474</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>918862</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Grafik 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{937F335B-640D-431E-93EA-39C8F4D14BE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20782178" y="11452412"/>
+          <a:ext cx="717590" cy="537862"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3141357</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4916137</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>615408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Grafik 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7488630F-5ABA-4AD9-AB1A-7A813B50BF17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20173248" y="12294254"/>
+          <a:ext cx="1774780" cy="536967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>26467</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>758780</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>658871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Grafik 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D4045B9-68F6-4F3B-A790-C3292B7F3B9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20779761" y="12326471"/>
+          <a:ext cx="732313" cy="546812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3260912</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>189635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4967678</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>706734</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Grafik 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79BBF503-0CCA-4393-8AE8-01C8CF41DDF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20282647" y="13166047"/>
+          <a:ext cx="1706766" cy="517099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>210652</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>703960</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>692541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Grafik 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0376DC93-D35D-4948-BA90-8E186BCF7EA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20798118" y="13187064"/>
+          <a:ext cx="659136" cy="481889"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>94481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4926214</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>719620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Grafik 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B74D9B50-F97D-4D84-B3B7-F24CD7933075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19879235" y="13832893"/>
+          <a:ext cx="2068714" cy="625139"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57388</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>212911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>670892</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>659475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Grafik 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2163DFCB-36B1-4539-A48E-5117E2484188}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20810682" y="13951323"/>
+          <a:ext cx="613504" cy="446564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2756646</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>96556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4719471</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>701696</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Grafik 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD532A88-4BF3-49FE-9B70-0202A2C0BF38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19778381" y="14596968"/>
+          <a:ext cx="1962825" cy="605140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>51903</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>737550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>655563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Grafik 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C190C06A-EADB-48EF-A67B-124E7DD4948B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20805197" y="14634883"/>
+          <a:ext cx="685647" cy="521092"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2823883</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4740202</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>780136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Grafik 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F351AF-A780-45FD-B23F-4B87C2403D22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18590559" y="15452912"/>
+          <a:ext cx="1916319" cy="589636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>749598</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>705970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Grafik 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACBD2864-F232-464C-9406-E4BDE9DF0504}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22019559" y="15408088"/>
+          <a:ext cx="738392" cy="560294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2608510</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4762615</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>703375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Grafik 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67BD9CE3-90BF-44EA-8280-5BA85FD15778}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19648735" y="16256373"/>
+          <a:ext cx="2154105" cy="658552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7538</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>46723</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>783869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Grafik 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC00D6D6-705C-4529-B1E9-68F8B1CB4AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22015891" y="16405412"/>
+          <a:ext cx="801185" cy="593369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2958354</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>293620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4692020</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>824960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Grafik 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{015C03BB-663A-4F11-8C37-479E7E5F3A6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19980089" y="17651532"/>
+          <a:ext cx="1733666" cy="531340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>11805</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>268939</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>48981</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>844934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Grafik 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6396EDF8-8451-4111-BD59-4FC833E742A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22020158" y="17626851"/>
+          <a:ext cx="799176" cy="575995"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1298,10 +2462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64198553-D51E-46AF-AC40-57B6C76EC5C4}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1312,13 +2476,14 @@
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="74.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1344,25 +2509,31 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="45.75" customHeight="1">
+    <row r="2" spans="1:18" ht="45.75" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1385,23 +2556,26 @@
       <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2">
         <v>256</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1424,23 +2598,26 @@
       <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3">
         <v>256</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30">
+    <row r="4" spans="1:18" ht="30">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1463,40 +2640,45 @@
       <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4">
         <v>256</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:18">
+      <c r="A5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:16" ht="45">
+    <row r="6" spans="1:18" ht="45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1519,23 +2701,26 @@
       <c r="H6" t="s">
         <v>8</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6">
         <v>256</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="45">
+    <row r="7" spans="1:18" ht="45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1558,23 +2743,26 @@
       <c r="H7" t="s">
         <v>8</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7">
         <v>256</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>28</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="45">
+    <row r="8" spans="1:18" ht="45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1597,23 +2785,26 @@
       <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8">
         <v>256</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>32</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="30">
+    <row r="9" spans="1:18" ht="30">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1636,23 +2827,27 @@
       <c r="H9" t="s">
         <v>35</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9">
         <v>256</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="30">
+    <row r="10" spans="1:18" ht="30">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1675,17 +2870,20 @@
       <c r="H10" t="s">
         <v>35</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10">
         <v>256</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="30">
+    <row r="11" spans="1:18" ht="30">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -1708,23 +2906,26 @@
       <c r="H11" t="s">
         <v>8</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11">
         <v>256</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>32</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="30">
+    <row r="12" spans="1:18" ht="30">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1747,23 +2948,26 @@
       <c r="H12" t="s">
         <v>8</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12">
         <v>256</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30">
+    <row r="13" spans="1:18" ht="30">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1786,23 +2990,26 @@
       <c r="H13" t="s">
         <v>8</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13">
         <v>256</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>32</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="45">
+    <row r="14" spans="1:18" ht="45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1827,23 +3034,26 @@
       <c r="H14" t="s">
         <v>8</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14">
         <v>256</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>48</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="O14" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="45">
+    <row r="15" spans="1:18" ht="45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1868,23 +3078,26 @@
       <c r="H15" t="s">
         <v>8</v>
       </c>
-      <c r="I15">
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15">
         <v>256</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>32</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="45">
+    <row r="16" spans="1:18" ht="45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1909,23 +3122,26 @@
       <c r="H16" t="s">
         <v>8</v>
       </c>
-      <c r="I16">
+      <c r="I16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16">
         <v>256</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>32</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>52</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="O16" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30">
+    <row r="17" spans="1:15" ht="30">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1947,23 +3163,26 @@
       <c r="H17" t="s">
         <v>8</v>
       </c>
-      <c r="I17">
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17">
         <v>256</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>32</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30">
+    <row r="18" spans="1:15" ht="30">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1985,23 +3204,27 @@
       <c r="H18" t="s">
         <v>35</v>
       </c>
-      <c r="I18">
+      <c r="I18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18">
         <v>256</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="9">
+      <c r="M18" s="9">
         <v>15685</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="N18" s="9"/>
+      <c r="O18" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:15" ht="30">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2023,25 +3246,600 @@
       <c r="H19" t="s">
         <v>8</v>
       </c>
-      <c r="I19">
+      <c r="I19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19">
         <v>256</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>55</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="O19" s="4" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+    </row>
+    <row r="21" spans="1:15" ht="45">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44337</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21">
+        <v>256</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="10">
+        <v>-0.25019999999999998</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="45">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22">
+        <v>256</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="11">
+        <v>-1.9850000000000001</v>
+      </c>
+      <c r="N22" s="11"/>
+      <c r="O22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="45">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23">
+        <v>256</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="11">
+        <v>-1.982</v>
+      </c>
+      <c r="N23" s="11"/>
+      <c r="O23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="45">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24">
+        <v>256</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="11">
+        <v>-1.982</v>
+      </c>
+      <c r="N24" s="11"/>
+      <c r="O24" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="45">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25">
+        <v>256</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="11">
+        <v>-1.9850000000000001</v>
+      </c>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="90">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26">
+        <v>256</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="11">
+        <v>-1.9862</v>
+      </c>
+      <c r="N26" s="11"/>
+      <c r="O26" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="60">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27">
+        <v>256</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="11">
+        <v>-1.9849000000000001</v>
+      </c>
+      <c r="N27" s="12">
+        <v>0.72389999999999999</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="60">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28">
+        <v>256</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="11">
+        <v>-1.9884999999999999</v>
+      </c>
+      <c r="N28" s="11"/>
+      <c r="O28" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="60">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29">
+        <v>256</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" s="11">
+        <v>-1.9881</v>
+      </c>
+      <c r="N29" s="12">
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="60">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30">
+        <v>256</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" s="11">
+        <v>-1.9887999999999999</v>
+      </c>
+      <c r="N30" s="12">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="75">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31">
+        <v>256</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" s="11">
+        <v>-1.9823</v>
+      </c>
+      <c r="N31" s="12">
+        <v>0.64429999999999998</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="90">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44340</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32">
+        <v>256</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="11">
+        <v>-1.9781</v>
+      </c>
+      <c r="N32" s="12">
+        <v>0.56010000000000004</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="90">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44341</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J33">
+        <v>256</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" s="11">
+        <v>-1.9759</v>
+      </c>
+      <c r="N33" s="12">
+        <v>0.54190000000000005</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A5:M5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A20:O20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>